<commit_message>
messing around with methodology for vector-multiplication calculation of species sensitivity based on traits
</commit_message>
<xml_diff>
--- a/_raw_data/cat_val_key_auto.xlsx
+++ b/_raw_data/cat_val_key_auto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="380" windowWidth="27280" windowHeight="15000"/>
+    <workbookView xWindow="2560" yWindow="3880" windowWidth="27280" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="valid_values" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t>Category</t>
   </si>
@@ -539,6 +539,95 @@
   </si>
   <si>
     <t>category_values</t>
+  </si>
+  <si>
+    <t>sessile; nearly sessile/sedentary; passive; vertical migrator; mobile resident; horizontal migrator; nomadic</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;1 day; &lt;1 week; &lt;1 month; &lt;4 months; 4 months -1yr; &gt;1yr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; not larvae</t>
+    </r>
+  </si>
+  <si>
+    <t>sexual dioecious; sexual hermaphrodite; asexual; colonial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-2; 2-5; 5-10; 10-20; 20-50; 50-100; 100-1000; 1000-10,000; &gt;10,000</t>
+  </si>
+  <si>
+    <t>1; 2-10; 11-25; 26-50; 51-100; 100+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">live birth/ egg care; spawner; egg-layer </t>
+  </si>
+  <si>
+    <t>feeding; non-feeding; no larva; NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;1000; 1K-10K; 10K-100K; 100K-1M; &gt;1M </t>
+  </si>
+  <si>
+    <t>yes; no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;7.4; 7.5-7.7; 7.8-8.2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitive; not sensitive; NA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">floating; yes; no </t>
+  </si>
+  <si>
+    <t>habitat list</t>
+  </si>
+  <si>
+    <t>specialist; generalist</t>
+  </si>
+  <si>
+    <t>one; few; many; does not aggregate</t>
+  </si>
+  <si>
+    <t>very small; small; medium; large</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;99</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; 100-4999; 5000-19,999; &gt;20,000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">epipelagic; mesopelagic; bathypelagic; abyssopelagic; hadopelagic </t>
+  </si>
+  <si>
+    <t>none; internal; external with a cover; external; in external protein matrix; in cellulose cell wall</t>
+  </si>
+  <si>
+    <t>none; larvae; adult; both</t>
+  </si>
+  <si>
+    <t>lungs; gills; skin; diffusion; pneumatophores; filter feeders</t>
+  </si>
+  <si>
+    <t>category_values2</t>
   </si>
 </sst>
 </file>
@@ -686,7 +775,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -703,6 +792,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1024,7 +1124,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1034,14 +1134,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="44.83203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="56.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="95.5" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1054,12 +1155,15 @@
       <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="12" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
@@ -1075,6 +1179,9 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="D4" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
@@ -1084,6 +1191,9 @@
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3"/>
@@ -1103,6 +1213,9 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
@@ -1112,6 +1225,9 @@
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D9" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
@@ -1121,6 +1237,9 @@
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D10" s="15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
@@ -1130,6 +1249,9 @@
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="16" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
@@ -1139,6 +1261,9 @@
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="D12" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
@@ -1148,6 +1273,9 @@
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D13" s="15" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
@@ -1157,6 +1285,9 @@
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D14" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
@@ -1166,6 +1297,9 @@
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D15" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
@@ -1175,8 +1309,11 @@
       <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>24</v>
@@ -1184,8 +1321,11 @@
       <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -1193,18 +1333,21 @@
       <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
@@ -1214,8 +1357,11 @@
       <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -1223,8 +1369,11 @@
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>33</v>
@@ -1232,8 +1381,11 @@
       <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>35</v>
@@ -1241,8 +1393,11 @@
       <c r="C24" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>37</v>
@@ -1250,8 +1405,11 @@
       <c r="C25" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>39</v>
@@ -1259,8 +1417,11 @@
       <c r="C26" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1268,8 +1429,11 @@
       <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1277,8 +1441,11 @@
       <c r="C28" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -1286,8 +1453,11 @@
       <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -1295,8 +1465,11 @@
       <c r="C30" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -1304,8 +1477,11 @@
       <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1313,8 +1489,11 @@
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
@@ -1322,8 +1501,11 @@
       <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
@@ -1333,8 +1515,11 @@
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>54</v>
@@ -1342,8 +1527,11 @@
       <c r="C35" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>56</v>
@@ -1351,8 +1539,11 @@
       <c r="C36" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>57</v>
       </c>
@@ -1362,8 +1553,11 @@
       <c r="C37" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>54</v>
@@ -1371,8 +1565,11 @@
       <c r="C38" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
         <v>56</v>
@@ -1380,18 +1577,21 @@
       <c r="C39" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="16">
+    <row r="42" spans="1:4" ht="16">
       <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
@@ -1399,8 +1599,11 @@
       <c r="C42" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>100</v>
       </c>
@@ -1408,8 +1611,11 @@
       <c r="C43" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
@@ -1417,18 +1623,21 @@
       <c r="C44" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>65</v>
       </c>
@@ -1436,8 +1645,11 @@
       <c r="C47" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -1445,8 +1657,11 @@
       <c r="C48" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
@@ -1454,8 +1669,11 @@
       <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>70</v>
       </c>
@@ -1463,8 +1681,11 @@
       <c r="C50" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
@@ -1472,8 +1693,11 @@
       <c r="C51" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>72</v>
       </c>
@@ -1481,8 +1705,11 @@
       <c r="C52" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>101</v>
       </c>
@@ -1490,8 +1717,11 @@
       <c r="C53" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>73</v>
       </c>
@@ -1499,8 +1729,11 @@
       <c r="C54" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>75</v>
       </c>
@@ -1508,24 +1741,27 @@
       <c r="C55" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D55" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:3" ht="15">
+    <row r="59" spans="1:4" ht="15">
       <c r="A59" s="11"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="A62" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64" s="10" t="s">
         <v>78</v>
       </c>

</xml_diff>